<commit_message>
No longer require estop reset after microswitch trip.  Rearrange modbus regs for simpler reads.
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="138">
   <si>
     <t>Register</t>
   </si>
@@ -209,6 +209,138 @@
     <t>Green LED pin state</t>
   </si>
   <si>
+    <t>MB_INWARD_ENDSTOP_STATE_DEPRECATED</t>
+  </si>
+  <si>
+    <t>MB_OUTWARD_ENDSTOP_STATE_DEPRECATED</t>
+  </si>
+  <si>
+    <t>MB_MOTOR_SETPOINT,</t>
+  </si>
+  <si>
+    <t>Motor speed setpoint (-ve is reverse)</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>{-100, 100}</t>
+  </si>
+  <si>
+    <t>Limited to +/-90% in test code</t>
+  </si>
+  <si>
+    <t>MB_MOTOR_SPEED,</t>
+  </si>
+  <si>
+    <t>Current motor speed</t>
+  </si>
+  <si>
+    <t>MB_MOTOR_ACCEL,</t>
+  </si>
+  <si>
+    <t>Current motor acceleration setting</t>
+  </si>
+  <si>
+    <t>ms/%</t>
+  </si>
+  <si>
+    <t>{0, 100}</t>
+  </si>
+  <si>
+    <t>MB_CURRENT_LIMIT_INWARD,</t>
+  </si>
+  <si>
+    <t>Current limit while running in reverse</t>
+  </si>
+  <si>
+    <t>{0, 8000}</t>
+  </si>
+  <si>
+    <t>MB_CURRENT_LIMIT_OUTWARD,</t>
+  </si>
+  <si>
+    <t>Current limit while running forward</t>
+  </si>
+  <si>
+    <t>MB_CURRENT_TRIPS_INWARD_DEPRECATED,</t>
+  </si>
+  <si>
+    <t>MB_CURRENT_TRIPS_OUTWARD_DEPRECATED,</t>
+  </si>
+  <si>
+    <t>MB_VOLTAGE_TRIPS_DEPRECATED,</t>
+  </si>
+  <si>
+    <t>MB_ESTOP,</t>
+  </si>
+  <si>
+    <t>Write anything to trigger emergency stop</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>MB_RESET_ESTOP,</t>
+  </si>
+  <si>
+    <t>Write 0x5050 to reset emergency stop</t>
+  </si>
+  <si>
+    <t>MB_MOTOR_PWM_FREQ_MSW,</t>
+  </si>
+  <si>
+    <t>Motor PWM frequency MSW</t>
+  </si>
+  <si>
+    <t>MB_MOTOR_PWM_FREQ_LSW,</t>
+  </si>
+  <si>
+    <t>Motor PWM frequency LSW</t>
+  </si>
+  <si>
+    <t>MB_MOTOR_PWM_DUTY_MSW,</t>
+  </si>
+  <si>
+    <t>Motor PWM duty cycle MSW</t>
+  </si>
+  <si>
+    <t>MB_MOTOR_PWM_DUTY_LSW,</t>
+  </si>
+  <si>
+    <t>Motor PWM duty cycle LSW</t>
+  </si>
+  <si>
+    <t>MB_INWARD_ENDSTOP_COUNT_DEPRECATED,</t>
+  </si>
+  <si>
+    <t>MB_OUTWARD_ENDSTOP_COUNT_DEPRECATED,</t>
+  </si>
+  <si>
+    <t>MB_HEARTBEAT_EXPIRIES_DEPRECATED</t>
+  </si>
+  <si>
+    <t>MB_ESTOP_STATE,</t>
+  </si>
+  <si>
+    <t>High if emergency stop has been triggered</t>
+  </si>
+  <si>
+    <t>Cleared when MB_RESET_ESTOP activated</t>
+  </si>
+  <si>
+    <t>MB_CURRENT_TRIPS_INWARD,</t>
+  </si>
+  <si>
+    <t>Number of current trips in reverse since boot</t>
+  </si>
+  <si>
+    <t>MB_CURRENT_TRIPS_OUTWARD,</t>
+  </si>
+  <si>
+    <t>Number of current trips in forward since boot</t>
+  </si>
+  <si>
     <t>MB_INWARD_ENDSTOP_STATE</t>
   </si>
   <si>
@@ -224,64 +356,16 @@
     <t>State of outward endstop microswitch</t>
   </si>
   <si>
-    <t>MB_MOTOR_SETPOINT,</t>
-  </si>
-  <si>
-    <t>Motor speed setpoint (-ve is reverse)</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>{-100, 100}</t>
-  </si>
-  <si>
-    <t>Limited to +/-90% in test code</t>
-  </si>
-  <si>
-    <t>MB_MOTOR_SPEED,</t>
-  </si>
-  <si>
-    <t>Current motor speed</t>
-  </si>
-  <si>
-    <t>MB_MOTOR_ACCEL,</t>
-  </si>
-  <si>
-    <t>Current motor acceleration setting</t>
-  </si>
-  <si>
-    <t>ms/%</t>
-  </si>
-  <si>
-    <t>{0, 100}</t>
-  </si>
-  <si>
-    <t>MB_CURRENT_LIMIT_INWARD,</t>
-  </si>
-  <si>
-    <t>Current limit while running in reverse</t>
-  </si>
-  <si>
-    <t>{0, 8000}</t>
-  </si>
-  <si>
-    <t>MB_CURRENT_LIMIT_OUTWARD,</t>
-  </si>
-  <si>
-    <t>Current limit while running forward</t>
-  </si>
-  <si>
-    <t>MB_CURRENT_TRIPS_INWARD,</t>
-  </si>
-  <si>
-    <t>Number of current trips in reverse since boot</t>
-  </si>
-  <si>
-    <t>MB_CURRENT_TRIPS_OUTWARD,</t>
-  </si>
-  <si>
-    <t>Number of current trips in forward since boot</t>
+    <t>MB_INWARD_ENDSTOP_COUNT,</t>
+  </si>
+  <si>
+    <t>Number of stops caused by inward endstop</t>
+  </si>
+  <si>
+    <t>MB_OUTWARD_ENDSTOP_COUNT,</t>
+  </si>
+  <si>
+    <t>Number of stops caused by outward endstop</t>
   </si>
   <si>
     <t>MB_VOLTAGE_TRIPS,</t>
@@ -290,55 +374,10 @@
     <t>Number of voltage limit trips since boot</t>
   </si>
   <si>
-    <t>MB_ESTOP,</t>
-  </si>
-  <si>
-    <t>Write anything to trigger emergency stop</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>MB_RESET_ESTOP,</t>
-  </si>
-  <si>
-    <t>Write 0x5050 to reset emergency stop</t>
-  </si>
-  <si>
-    <t>MB_MOTOR_PWM_FREQ_MSW,</t>
-  </si>
-  <si>
-    <t>Motor PWM frequency MSW</t>
-  </si>
-  <si>
-    <t>MB_MOTOR_PWM_FREQ_LSW,</t>
-  </si>
-  <si>
-    <t>Motor PWM frequency LSW</t>
-  </si>
-  <si>
-    <t>MB_MOTOR_PWM_DUTY_MSW,</t>
-  </si>
-  <si>
-    <t>Motor PWM duty cycle MSW</t>
-  </si>
-  <si>
-    <t>MB_MOTOR_PWM_DUTY_LSW,</t>
-  </si>
-  <si>
-    <t>Motor PWM duty cycle LSW</t>
-  </si>
-  <si>
-    <t>MB_INWARD_ENDSTOP_COUNT,</t>
-  </si>
-  <si>
-    <t>Number of stops caused by inward endstop</t>
-  </si>
-  <si>
-    <t>MB_OUTWARD_ENDSTOP_COUNT,</t>
-  </si>
-  <si>
-    <t>Number of stops caused by outward endstop</t>
+    <t>MB_HEARTBEAT_EXPIRIES</t>
+  </si>
+  <si>
+    <t>Number of trips caused by heartbeat timer expiry</t>
   </si>
   <si>
     <t>MB_UNLOCK_CONFIG,</t>
@@ -516,19 +555,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A18" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="A28" activeCellId="0" pane="topLeft" sqref="A28"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="B46" activeCellId="0" pane="topLeft" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1785714285714"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.0357142857143"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.4387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -952,37 +991,13 @@
       <c r="B27" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
         <v>116</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
@@ -990,22 +1005,22 @@
         <v>200</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
@@ -1013,19 +1028,19 @@
         <v>201</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
@@ -1033,19 +1048,19 @@
         <v>202</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
@@ -1053,10 +1068,10 @@
         <v>203</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>3</v>
@@ -1065,7 +1080,7 @@
         <v>30</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
@@ -1073,10 +1088,10 @@
         <v>204</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>3</v>
@@ -1085,7 +1100,7 @@
         <v>30</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
@@ -1093,13 +1108,7 @@
         <v>205</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
@@ -1107,13 +1116,7 @@
         <v>206</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
@@ -1121,13 +1124,7 @@
         <v>207</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
@@ -1135,13 +1132,13 @@
         <v>208</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
@@ -1149,13 +1146,13 @@
         <v>209</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
@@ -1163,10 +1160,10 @@
         <v>210</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>9</v>
@@ -1177,10 +1174,10 @@
         <v>211</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>9</v>
@@ -1191,10 +1188,10 @@
         <v>212</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>9</v>
@@ -1205,10 +1202,10 @@
         <v>213</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>9</v>
@@ -1219,13 +1216,7 @@
         <v>214</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
@@ -1233,163 +1224,309 @@
         <v>215</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
-      <c r="A47" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>36</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+      <c r="A46" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="n">
-        <v>9001</v>
+        <v>300</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="n">
-        <v>9002</v>
+        <v>301</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="n">
-        <v>9003</v>
+        <v>302</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="n">
-        <v>9004</v>
+        <v>303</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>3</v>
+        <v>109</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="n">
-        <v>9005</v>
+        <v>304</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>3</v>
+        <v>112</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="n">
-        <v>9006</v>
+        <v>305</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
+        <v>306</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
+      <c r="A55" s="0" t="n">
+        <v>307</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+      <c r="A56" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+      <c r="A58" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+      <c r="A59" s="0" t="n">
+        <v>9001</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
+      <c r="A60" s="0" t="n">
+        <v>9002</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+      <c r="A61" s="0" t="n">
+        <v>9003</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
+      <c r="A62" s="0" t="n">
+        <v>9004</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
+      <c r="A63" s="0" t="n">
+        <v>9005</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
+      <c r="A64" s="0" t="n">
+        <v>9006</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
+      <c r="A65" s="0" t="n">
         <v>9007</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D54" s="0" t="s">
+      <c r="B65" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D65" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E65" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G54" s="0" t="s">
+      <c r="G65" s="0" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add quadrature encoder input for position, multiplexed with inward endstop switch
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="134" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="95" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="141">
   <si>
     <t>Register</t>
   </si>
@@ -213,6 +213,15 @@
   </si>
   <si>
     <t>MB_OUTWARD_ENDSTOP_STATE_DEPRECATED</t>
+  </si>
+  <si>
+    <t>MB_POSITION_ENCODER_COUNTS</t>
+  </si>
+  <si>
+    <t>Counts of position encoder</t>
+  </si>
+  <si>
+    <t>Signed</t>
   </si>
   <si>
     <t>MB_MOTOR_SETPOINT,</t>
@@ -555,10 +564,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="B46" activeCellId="0" pane="topLeft" sqref="B46"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="A29" activeCellId="0" pane="topLeft" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1000,84 +1009,81 @@
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
-      <c r="A30" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="B30" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C29" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="D29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="F31" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>69</v>
+      <c r="G31" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="n">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>78</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>79</v>
@@ -1085,7 +1091,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="n">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>80</v>
@@ -1100,50 +1106,56 @@
         <v>30</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="n">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="n">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="n">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="n">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="0" t="s">
         <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="n">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>88</v>
@@ -1152,32 +1164,32 @@
         <v>89</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="n">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="n">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>9</v>
@@ -1185,13 +1197,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="n">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>9</v>
@@ -1199,13 +1211,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="n">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>9</v>
@@ -1213,51 +1225,45 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="n">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="0" t="n">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+      <c r="A47" s="0" t="n">
         <v>216</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
-      <c r="A48" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G48" s="0" t="s">
+      <c r="B47" s="0" t="s">
         <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="n">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>104</v>
@@ -1268,16 +1274,22 @@
       <c r="D49" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="E49" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="n">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>9</v>
@@ -1285,27 +1297,21 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="n">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51" s="0" t="s">
         <v>110</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="n">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>111</v>
@@ -1313,39 +1319,45 @@
       <c r="C52" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>49</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="n">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G53" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>9</v>
@@ -1353,13 +1365,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="n">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>9</v>
@@ -1367,50 +1379,44 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
+        <v>307</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
+      <c r="A57" s="0" t="n">
         <v>308</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
-      <c r="A58" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58" s="0" t="s">
+      <c r="B57" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G58" s="0" t="s">
-        <v>36</v>
+      <c r="C57" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="n">
-        <v>9001</v>
+        <v>9000</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>36</v>
@@ -1418,7 +1424,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="n">
-        <v>9002</v>
+        <v>9001</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>126</v>
@@ -1429,19 +1435,22 @@
       <c r="D60" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E60" s="0" t="s">
+        <v>128</v>
+      </c>
       <c r="G60" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="n">
-        <v>9003</v>
+        <v>9002</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>3</v>
@@ -1452,33 +1461,30 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="0" t="n">
-        <v>9004</v>
+        <v>9003</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E62" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="G62" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
-        <v>9005</v>
+        <v>9004</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>3</v>
@@ -1492,13 +1498,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="0" t="n">
-        <v>9006</v>
+        <v>9005</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>3</v>
@@ -1512,13 +1518,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="n">
-        <v>9007</v>
+        <v>9006</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>3</v>
@@ -1527,6 +1533,26 @@
         <v>30</v>
       </c>
       <c r="G65" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
+      <c r="A66" s="0" t="n">
+        <v>9007</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="0" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add configurable extension limits
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="155">
   <si>
     <t>Register</t>
   </si>
@@ -221,7 +221,7 @@
     <t>Counts of position encoder</t>
   </si>
   <si>
-    <t>Signed</t>
+    <t>Signed, returns 0x7FFF if uncalibrated</t>
   </si>
   <si>
     <t>MB_MOTOR_SETPOINT,</t>
@@ -272,10 +272,25 @@
     <t>Current limit while running forward</t>
   </si>
   <si>
-    <t>MB_CURRENT_TRIPS_INWARD_DEPRECATED,</t>
-  </si>
-  <si>
-    <t>MB_CURRENT_TRIPS_OUTWARD_DEPRECATED,</t>
+    <t>MB_EXTENSION_LIMIT_INWARD,</t>
+  </si>
+  <si>
+    <t>Maximum inward extension</t>
+  </si>
+  <si>
+    <t>0.1 mm</t>
+  </si>
+  <si>
+    <t>Must be less than zero or will be unable to calibrate. Formerly MB_CURRENT_TRIPS_INWARD_DEPRECATED,</t>
+  </si>
+  <si>
+    <t>MB_EXTENSION_LIMIT_OUTWARD,</t>
+  </si>
+  <si>
+    <t>Maximum outward extension</t>
+  </si>
+  <si>
+    <t>Formerly MB_CURRENT_TRIPS_OUTWARD_DEPRECATED,</t>
   </si>
   <si>
     <t>MB_VOLTAGE_TRIPS_DEPRECATED,</t>
@@ -326,7 +341,22 @@
     <t>MB_OUTWARD_ENDSTOP_COUNT_DEPRECATED,</t>
   </si>
   <si>
-    <t>MB_HEARTBEAT_EXPIRIES_DEPRECATED</t>
+    <t>MB_HEARTBEAT_EXPIRIES_DEPRECATED,</t>
+  </si>
+  <si>
+    <t>MB_POSITION_ENCODER_SCALING,</t>
+  </si>
+  <si>
+    <t>Tenths of a mm extension per position encoder count</t>
+  </si>
+  <si>
+    <t>0.1mm / count</t>
+  </si>
+  <si>
+    <t>MB_EXTENSION,</t>
+  </si>
+  <si>
+    <t>Extension distance, as measured by position encoder</t>
   </si>
   <si>
     <t>MB_ESTOP_STATE,</t>
@@ -383,10 +413,22 @@
     <t>Number of voltage limit trips since boot</t>
   </si>
   <si>
-    <t>MB_HEARTBEAT_EXPIRIES</t>
+    <t>MB_HEARTBEAT_EXPIRIES,</t>
   </si>
   <si>
     <t>Number of trips caused by heartbeat timer expiry</t>
+  </si>
+  <si>
+    <t>MB_EXTENSION_TRIPS_INWARD,</t>
+  </si>
+  <si>
+    <t>Number of trips caused by exceeding inward extension limit</t>
+  </si>
+  <si>
+    <t>MB_EXTENSION_TRIPS_OUTWARD,</t>
+  </si>
+  <si>
+    <t>Number of trips caused by exceeding Outward extension limit</t>
   </si>
   <si>
     <t>MB_UNLOCK_CONFIG,</t>
@@ -564,10 +606,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="A29" activeCellId="0" pane="topLeft" sqref="A29"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B24" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="B29" activeCellId="0" pane="topLeft" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -575,8 +617,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1785714285714"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.0357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.3775510204082"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -1136,13 +1180,37 @@
       <c r="B36" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="C36" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="n">
         <v>206</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
@@ -1150,7 +1218,7 @@
         <v>207</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
@@ -1158,13 +1226,13 @@
         <v>208</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
@@ -1172,13 +1240,13 @@
         <v>209</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
@@ -1186,10 +1254,10 @@
         <v>210</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>9</v>
@@ -1200,10 +1268,10 @@
         <v>211</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>9</v>
@@ -1214,10 +1282,10 @@
         <v>212</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>9</v>
@@ -1228,10 +1296,10 @@
         <v>213</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>9</v>
@@ -1242,7 +1310,7 @@
         <v>214</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
@@ -1250,7 +1318,7 @@
         <v>215</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
@@ -1258,134 +1326,143 @@
         <v>216</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
-      <c r="A49" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
+      <c r="A48" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="n">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="n">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="n">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="n">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>113</v>
+        <v>120</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>9</v>
+        <v>122</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="n">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>9</v>
+        <v>125</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>9</v>
@@ -1393,104 +1470,86 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="n">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D57" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+      <c r="A58" s="0" t="n">
+        <v>307</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D58" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="n">
-        <v>9000</v>
+        <v>308</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G59" s="0" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="n">
-        <v>9001</v>
+        <v>309</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="G60" s="0" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="n">
-        <v>9002</v>
+        <v>310</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="G61" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
-      <c r="A62" s="0" t="n">
-        <v>9003</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
-        <v>9004</v>
+        <v>9000</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="G63" s="0" t="s">
         <v>36</v>
@@ -1498,19 +1557,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="0" t="n">
-        <v>9005</v>
+        <v>9001</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="G64" s="0" t="s">
         <v>36</v>
@@ -1518,44 +1577,120 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="n">
-        <v>9006</v>
+        <v>9002</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E65" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="G65" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="0" t="n">
-        <v>9007</v>
+        <v>9003</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="G66" s="0" t="s">
         <v>36</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
+      <c r="A67" s="0" t="n">
+        <v>9004</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
+      <c r="A68" s="0" t="n">
+        <v>9005</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
+      <c r="A69" s="0" t="n">
+        <v>9006</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
+      <c r="A70" s="0" t="n">
+        <v>9007</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048575"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add goto position command
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="161">
   <si>
     <t>Register</t>
   </si>
@@ -351,6 +351,24 @@
   </si>
   <si>
     <t>0.1mm / count</t>
+  </si>
+  <si>
+    <t>MB_GOTO_POSITION,</t>
+  </si>
+  <si>
+    <t>Command to manually move to a position, at gotoSpeedSetpoint</t>
+  </si>
+  <si>
+    <t>Signed. Actuator will move at setpoint speed in either direction.  Returns 0x7FFF if no position set/clears to this value on completion</t>
+  </si>
+  <si>
+    <t>MB_GOTO_SPEED_SETPOINT,</t>
+  </si>
+  <si>
+    <t>Speed to run at when goto command running</t>
+  </si>
+  <si>
+    <t>{1, 100}</t>
   </si>
   <si>
     <t>MB_EXTENSION,</t>
@@ -606,17 +624,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B24" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="B29" activeCellId="0" pane="topLeft" sqref="B29"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A20" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="C50" activeCellId="0" pane="topLeft" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.8367346938776"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1632653061225"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
@@ -1346,151 +1364,163 @@
         <v>111</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+      <c r="A49" s="0" t="n">
+        <v>218</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="n">
-        <v>299</v>
+        <v>219</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
-      <c r="A51" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>116</v>
+        <v>71</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="n">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="n">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G54" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="n">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G55" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>9</v>
+        <v>128</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="n">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C57" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G57" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="n">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>9</v>
@@ -1498,13 +1528,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="n">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>9</v>
@@ -1512,13 +1542,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="n">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>9</v>
@@ -1526,67 +1556,58 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="n">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D61" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
+      <c r="A62" s="0" t="n">
+        <v>309</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
-        <v>9000</v>
+        <v>310</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
-      <c r="A64" s="0" t="n">
-        <v>9001</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="n">
-        <v>9002</v>
+        <v>9000</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="G65" s="0" t="s">
         <v>36</v>
@@ -1594,16 +1615,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="0" t="n">
-        <v>9003</v>
+        <v>9001</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>148</v>
       </c>
       <c r="G66" s="0" t="s">
         <v>36</v>
@@ -1611,19 +1635,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="0" t="n">
-        <v>9004</v>
+        <v>9002</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="G67" s="0" t="s">
         <v>36</v>
@@ -1631,19 +1652,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="n">
-        <v>9005</v>
+        <v>9003</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>36</v>
@@ -1651,13 +1669,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="n">
-        <v>9006</v>
+        <v>9004</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>3</v>
@@ -1671,13 +1689,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="n">
-        <v>9007</v>
+        <v>9005</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>3</v>
@@ -1689,8 +1707,46 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048575"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
+      <c r="A71" s="0" t="n">
+        <v>9006</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
+      <c r="A72" s="0" t="n">
+        <v>9007</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Position encoder backward compatibility
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -293,7 +293,16 @@
     <t>Formerly MB_CURRENT_TRIPS_OUTWARD_DEPRECATED,</t>
   </si>
   <si>
-    <t>MB_VOLTAGE_TRIPS_DEPRECATED,</t>
+    <t>MB_POSITION_ENCODER_SCALING,</t>
+  </si>
+  <si>
+    <t>Tenths of a mm extension per position encoder count</t>
+  </si>
+  <si>
+    <t>0.1mm / count</t>
+  </si>
+  <si>
+    <t>Set to zero to disable encoder. Formerly MB_VOLTAGE_TRIPS_DEPRECATED,</t>
   </si>
   <si>
     <t>MB_ESTOP,</t>
@@ -342,15 +351,6 @@
   </si>
   <si>
     <t>MB_HEARTBEAT_EXPIRIES_DEPRECATED,</t>
-  </si>
-  <si>
-    <t>MB_POSITION_ENCODER_SCALING,</t>
-  </si>
-  <si>
-    <t>Tenths of a mm extension per position encoder count</t>
-  </si>
-  <si>
-    <t>0.1mm / count</t>
   </si>
   <si>
     <t>MB_GOTO_POSITION,</t>
@@ -624,10 +624,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A20" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="C50" activeCellId="0" pane="topLeft" sqref="C50"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="A39" activeCellId="0" pane="topLeft" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1238,19 +1238,31 @@
       <c r="B38" s="0" t="s">
         <v>92</v>
       </c>
+      <c r="C38" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="n">
         <v>208</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
@@ -1258,13 +1270,13 @@
         <v>209</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
@@ -1272,10 +1284,10 @@
         <v>210</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>9</v>
@@ -1286,10 +1298,10 @@
         <v>211</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>9</v>
@@ -1300,10 +1312,10 @@
         <v>212</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>9</v>
@@ -1314,10 +1326,10 @@
         <v>213</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>9</v>
@@ -1328,7 +1340,7 @@
         <v>214</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
@@ -1336,7 +1348,7 @@
         <v>215</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
@@ -1344,25 +1356,13 @@
         <v>216</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="n">
         <v>217</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="n">
@@ -1607,7 +1607,7 @@
         <v>145</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G65" s="0" t="s">
         <v>36</v>
@@ -1747,6 +1747,7 @@
         <v>36</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add force calibrate function
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="163">
   <si>
     <t>Register</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>{1, 100}</t>
+  </si>
+  <si>
+    <t>MB_FORCE_CALIBRATE_ENCODER,</t>
+  </si>
+  <si>
+    <t>Write 0xA0A0 to force encoder to calibrate to zero in current position</t>
   </si>
   <si>
     <t>MB_EXTENSION,</t>
@@ -624,10 +630,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="A39" activeCellId="0" pane="topLeft" sqref="A39"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A35" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="E51" activeCellId="0" pane="topLeft" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1404,29 +1410,23 @@
         <v>117</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
-      <c r="A52" s="0" t="n">
-        <v>299</v>
-      </c>
-      <c r="B52" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
+      <c r="A51" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C51" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>68</v>
+      <c r="D51" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="n">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>120</v>
@@ -1438,29 +1438,35 @@
         <v>9</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B54" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="D54" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="n">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>125</v>
@@ -1474,7 +1480,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>127</v>
@@ -1482,39 +1488,33 @@
       <c r="C56" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G56" s="0" t="s">
-        <v>129</v>
+      <c r="D56" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="n">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>49</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="n">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>132</v>
@@ -1522,13 +1522,19 @@
       <c r="C58" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>9</v>
+      <c r="D58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="n">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>134</v>
@@ -1542,7 +1548,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="n">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>136</v>
@@ -1556,7 +1562,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="n">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>138</v>
@@ -1570,7 +1576,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="0" t="n">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>140</v>
@@ -1584,7 +1590,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>142</v>
@@ -1596,26 +1602,23 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
-      <c r="A65" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="B65" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
+      <c r="A64" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="B64" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C64" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G65" s="0" t="s">
-        <v>36</v>
+      <c r="D64" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="0" t="n">
-        <v>9001</v>
+        <v>9000</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>146</v>
@@ -1624,10 +1627,7 @@
         <v>147</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="G66" s="0" t="s">
         <v>36</v>
@@ -1635,16 +1635,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="0" t="n">
-        <v>9002</v>
+        <v>9001</v>
       </c>
       <c r="B67" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="D67" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>3</v>
       </c>
       <c r="G67" s="0" t="s">
         <v>36</v>
@@ -1652,7 +1655,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="n">
-        <v>9003</v>
+        <v>9002</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>151</v>
@@ -1669,7 +1672,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="n">
-        <v>9004</v>
+        <v>9003</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>153</v>
@@ -1680,16 +1683,13 @@
       <c r="D69" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="G69" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="n">
-        <v>9005</v>
+        <v>9004</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>155</v>
@@ -1709,7 +1709,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="0" t="n">
-        <v>9006</v>
+        <v>9005</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>157</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="0" t="n">
-        <v>9007</v>
+        <v>9006</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>159</v>
@@ -1747,7 +1747,26 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
+      <c r="A73" s="0" t="n">
+        <v>9007</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Minor version bump: v0.6 = encoder failure detection
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="170">
   <si>
     <t>Register</t>
   </si>
@@ -455,6 +455,12 @@
     <t>Number of trips caused by exceeding Outward extension limit</t>
   </si>
   <si>
+    <t>MB_ENCODER_FAIL_TRIPS,</t>
+  </si>
+  <si>
+    <t>Number of trips caused by encoder failure detection</t>
+  </si>
+  <si>
     <t>MB_UNLOCK_CONFIG,</t>
   </si>
   <si>
@@ -504,6 +510,21 @@
   </si>
   <si>
     <t>Max forward current limit</t>
+  </si>
+  <si>
+    <t>MB_HEARTBEAT_TIMEOUT,</t>
+  </si>
+  <si>
+    <t>Seconds before heartbeat timer expires</t>
+  </si>
+  <si>
+    <t>MB_ENCODER_FAIL_TIMEOUT,</t>
+  </si>
+  <si>
+    <t>Max milliseconds between encoder pulses before timeout</t>
+  </si>
+  <si>
+    <t>ms</t>
   </si>
 </sst>
 </file>
@@ -592,7 +613,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -613,6 +634,10 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -630,10 +655,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A35" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="E51" activeCellId="0" pane="topLeft" sqref="E51"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A42" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="E77" activeCellId="0" pane="topLeft" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1616,26 +1641,23 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
-      <c r="A66" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="B66" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
+      <c r="A65" s="0" t="n">
+        <v>311</v>
+      </c>
+      <c r="B65" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C65" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="D66" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G66" s="0" t="s">
-        <v>36</v>
+      <c r="D65" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="0" t="n">
-        <v>9001</v>
+        <v>9000</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>148</v>
@@ -1644,10 +1666,7 @@
         <v>149</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="G67" s="0" t="s">
         <v>36</v>
@@ -1655,16 +1674,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="n">
-        <v>9002</v>
+        <v>9001</v>
       </c>
       <c r="B68" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C68" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="D68" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>3</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>36</v>
@@ -1672,7 +1694,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="n">
-        <v>9003</v>
+        <v>9002</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>153</v>
@@ -1689,7 +1711,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="n">
-        <v>9004</v>
+        <v>9003</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>155</v>
@@ -1700,16 +1722,13 @@
       <c r="D70" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="G70" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="0" t="n">
-        <v>9005</v>
+        <v>9004</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>157</v>
@@ -1729,7 +1748,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="0" t="n">
-        <v>9006</v>
+        <v>9005</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>159</v>
@@ -1749,7 +1768,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="0" t="n">
-        <v>9007</v>
+        <v>9006</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>161</v>
@@ -1765,6 +1784,60 @@
       </c>
       <c r="G73" s="0" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
+      <c r="A74" s="0" t="n">
+        <v>9007</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
+      <c r="A75" s="0" t="n">
+        <v>9008</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
+      <c r="A76" s="0" t="n">
+        <v>9009</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert MB_ESTOP_STATE to enum stop reason
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="95" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="211" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Modbus Map" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="E-Stop Reasons" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="181">
   <si>
     <t>Register</t>
   </si>
@@ -386,10 +387,13 @@
     <t>MB_ESTOP_STATE,</t>
   </si>
   <si>
-    <t>High if emergency stop has been triggered</t>
-  </si>
-  <si>
-    <t>Cleared when MB_RESET_ESTOP activated</t>
+    <t>Status of emergency stop (first trip reason)</t>
+  </si>
+  <si>
+    <t>enumeration</t>
+  </si>
+  <si>
+    <t>See 'E-Stop Reasons' sheet.  Cleared when MB_RESET_ESTOP activated</t>
   </si>
   <si>
     <t>MB_CURRENT_TRIPS_INWARD,</t>
@@ -525,6 +529,36 @@
   </si>
   <si>
     <t>ms</t>
+  </si>
+  <si>
+    <t>E-Stop Reasons</t>
+  </si>
+  <si>
+    <t>NOT_ESTOPPED,</t>
+  </si>
+  <si>
+    <t>ESTOP_REMOTE_COMMAND,</t>
+  </si>
+  <si>
+    <t>ESTOP_CURRENT_LIMIT_INWARD,</t>
+  </si>
+  <si>
+    <t>ESTOP_CURRENT_LIMIT_OUTWARD,</t>
+  </si>
+  <si>
+    <t>ESTOP_BATT_OVERVOLTAGE,</t>
+  </si>
+  <si>
+    <t>ESTOP_EXTENSION_LIMIT_INWARD,</t>
+  </si>
+  <si>
+    <t>ESTOP_EXTENSION_LIMIT_OUTWARD,</t>
+  </si>
+  <si>
+    <t>ESTOP_ENCODER_FAILURE,</t>
+  </si>
+  <si>
+    <t>ESTOP_HEARTBEAT_TIMEOUT</t>
   </si>
 </sst>
 </file>
@@ -613,7 +647,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -638,6 +672,10 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -658,7 +696,7 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A42" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="E77" activeCellId="0" pane="topLeft" sqref="E77"/>
+      <selection activeCell="C54" activeCellId="0" pane="topLeft" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1483,10 +1521,10 @@
         <v>9</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
@@ -1494,10 +1532,10 @@
         <v>301</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>9</v>
@@ -1508,10 +1546,10 @@
         <v>302</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>9</v>
@@ -1522,10 +1560,10 @@
         <v>303</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>9</v>
@@ -1534,7 +1572,7 @@
         <v>49</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
@@ -1542,10 +1580,10 @@
         <v>304</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>9</v>
@@ -1554,7 +1592,7 @@
         <v>49</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
@@ -1562,10 +1600,10 @@
         <v>305</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>9</v>
@@ -1576,10 +1614,10 @@
         <v>306</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>9</v>
@@ -1590,10 +1628,10 @@
         <v>307</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>9</v>
@@ -1604,10 +1642,10 @@
         <v>308</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>9</v>
@@ -1618,10 +1656,10 @@
         <v>309</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>9</v>
@@ -1632,10 +1670,10 @@
         <v>310</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>9</v>
@@ -1646,10 +1684,10 @@
         <v>311</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>9</v>
@@ -1660,10 +1698,10 @@
         <v>9000</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>98</v>
@@ -1677,16 +1715,16 @@
         <v>9001</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>36</v>
@@ -1697,10 +1735,10 @@
         <v>9002</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>3</v>
@@ -1714,10 +1752,10 @@
         <v>9003</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>3</v>
@@ -1731,10 +1769,10 @@
         <v>9004</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>3</v>
@@ -1751,10 +1789,10 @@
         <v>9005</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>3</v>
@@ -1771,10 +1809,10 @@
         <v>9006</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>3</v>
@@ -1791,10 +1829,10 @@
         <v>9007</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>3</v>
@@ -1811,10 +1849,10 @@
         <v>9008</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>3</v>
@@ -1828,16 +1866,16 @@
         <v>9009</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1849,4 +1887,108 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="B2" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="B8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="B9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="B10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="B11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="B12" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit of combined Helios/Uki branch, including build variants for hardware type (Helios has analogue position encoder, digital endstops) and external ADC enable; also voltage measurement calibration, overtemperature trip and increased max current limit to 20A.
</commit_message>
<xml_diff>
--- a/Modbus map.xlsx
+++ b/Modbus map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="185">
   <si>
     <t>Register</t>
   </si>
@@ -354,6 +354,12 @@
     <t>MB_HEARTBEAT_EXPIRIES_DEPRECATED,</t>
   </si>
   <si>
+    <t>MB_TEMPERATURE_LIMIT</t>
+  </si>
+  <si>
+    <t>Overtemperature trip point</t>
+  </si>
+  <si>
     <t>MB_GOTO_POSITION,</t>
   </si>
   <si>
@@ -463,6 +469,12 @@
   </si>
   <si>
     <t>Number of trips caused by encoder failure detection</t>
+  </si>
+  <si>
+    <t>MB_TEMPERATURE_TRIPS,</t>
+  </si>
+  <si>
+    <t>Number of trips due to overtemperature</t>
   </si>
   <si>
     <t>MB_UNLOCK_CONFIG,</t>
@@ -660,16 +672,16 @@
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
@@ -693,10 +705,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A42" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
-      <selection activeCell="C54" activeCellId="0" pane="topLeft" sqref="C54"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A30" view="normal" windowProtection="false" workbookViewId="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100">
+      <selection activeCell="B48" activeCellId="0" pane="topLeft" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1432,16 +1444,28 @@
       <c r="A48" s="0" t="n">
         <v>217</v>
       </c>
+      <c r="B48" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="n">
         <v>218</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>3</v>
@@ -1450,7 +1474,7 @@
         <v>87</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
@@ -1458,10 +1482,10 @@
         <v>219</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>3</v>
@@ -1470,7 +1494,7 @@
         <v>71</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
@@ -1478,10 +1502,10 @@
         <v>220</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>98</v>
@@ -1492,10 +1516,10 @@
         <v>299</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>9</v>
@@ -1512,19 +1536,19 @@
         <v>300</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
@@ -1532,10 +1556,10 @@
         <v>301</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>9</v>
@@ -1546,10 +1570,10 @@
         <v>302</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>9</v>
@@ -1560,19 +1584,19 @@
         <v>303</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D57" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>49</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
@@ -1580,19 +1604,19 @@
         <v>304</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D58" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E58" s="0" t="s">
         <v>49</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
@@ -1600,10 +1624,10 @@
         <v>305</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>9</v>
@@ -1614,10 +1638,10 @@
         <v>306</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>9</v>
@@ -1628,10 +1652,10 @@
         <v>307</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>9</v>
@@ -1642,10 +1666,10 @@
         <v>308</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>9</v>
@@ -1656,10 +1680,10 @@
         <v>309</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>9</v>
@@ -1670,10 +1694,10 @@
         <v>310</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>9</v>
@@ -1684,47 +1708,41 @@
         <v>311</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
-      <c r="A67" s="0" t="n">
-        <v>9000</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>36</v>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
+      <c r="A66" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="n">
-        <v>9001</v>
+        <v>9000</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>153</v>
+        <v>98</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>36</v>
@@ -1732,16 +1750,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="n">
-        <v>9002</v>
+        <v>9001</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>157</v>
       </c>
       <c r="G69" s="0" t="s">
         <v>36</v>
@@ -1749,13 +1770,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="n">
-        <v>9003</v>
+        <v>9002</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>3</v>
@@ -1766,19 +1787,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="0" t="n">
-        <v>9004</v>
+        <v>9003</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>36</v>
@@ -1786,13 +1804,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="0" t="n">
-        <v>9005</v>
+        <v>9004</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>3</v>
@@ -1806,13 +1824,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="0" t="n">
-        <v>9006</v>
+        <v>9005</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>3</v>
@@ -1826,13 +1844,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="A74" s="0" t="n">
-        <v>9007</v>
+        <v>9006</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>3</v>
@@ -1846,36 +1864,56 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
       <c r="A75" s="0" t="n">
-        <v>9008</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>166</v>
+        <v>9007</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>168</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="A76" s="0" t="n">
+        <v>9008</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
+      <c r="A77" s="0" t="n">
         <v>9009</v>
       </c>
-      <c r="B76" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>170</v>
+      <c r="B77" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1907,7 +1945,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="B2" s="6" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
@@ -1915,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
@@ -1923,7 +1961,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -1931,7 +1969,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -1939,7 +1977,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -1947,7 +1985,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -1955,7 +1993,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
@@ -1963,7 +2001,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
@@ -1971,7 +2009,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
@@ -1979,7 +2017,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>